<commit_message>
partial config results ansible
</commit_message>
<xml_diff>
--- a/R/deploytimes/deploytimes.xlsx
+++ b/R/deploytimes/deploytimes.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas_2\Documents\Bachelorproef-Ansible-vs-Puppet\R\deploytimes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasdetemmerman/Documents/Bachelorproef-Ansible-vs-Puppet/R/deploytimes/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16035" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16040" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Puppet" sheetId="1" r:id="rId1"/>
     <sheet name="Ansible" sheetId="2" r:id="rId2"/>
-    <sheet name="grafiek" sheetId="3" r:id="rId3"/>
+    <sheet name="Ansible partial config" sheetId="5" r:id="rId3"/>
+    <sheet name="grafiek" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="62">
   <si>
     <t>total</t>
   </si>
@@ -201,16 +202,31 @@
   <si>
     <t>n</t>
   </si>
+  <si>
+    <t>changed in config</t>
+  </si>
+  <si>
+    <t>mariadb running</t>
+  </si>
+  <si>
+    <t>lorem ipsum</t>
+  </si>
+  <si>
+    <t>ANSIBLE</t>
+  </si>
+  <si>
+    <t>Puppet</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -286,9 +302,17 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="32">
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -401,7 +425,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
@@ -465,7 +489,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -511,7 +535,7 @@
                   <c:v>5.68</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>11.18</c:v>
@@ -559,45 +583,45 @@
                   <c:v>8.23</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>7.41</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A7F8-4E2E-B041-79643940DA82}"/>
             </c:ext>
@@ -645,7 +669,7 @@
                   <c:v>55.18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.590000000000003</c:v>
+                  <c:v>40.59</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>47.01</c:v>
@@ -725,7 +749,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-A7F8-4E2E-B041-79643940DA82}"/>
             </c:ext>
@@ -739,11 +763,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2077638544"/>
-        <c:axId val="2122137344"/>
+        <c:axId val="680117488"/>
+        <c:axId val="680119264"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-2077638544"/>
+        <c:axId val="680117488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -782,10 +806,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2122137344"/>
+        <c:crossAx val="680119264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -793,7 +817,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2122137344"/>
+        <c:axId val="680119264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -841,10 +865,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2077638544"/>
+        <c:crossAx val="680117488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -883,7 +907,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -913,7 +937,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-BE"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -925,7 +949,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
@@ -968,8 +992,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.40352777777777799"/>
-          <c:y val="4.6296296296296301E-2"/>
+          <c:x val="0.403527777777778"/>
+          <c:y val="0.0462962962962963"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -997,7 +1021,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1008,10 +1032,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.9636482939632501E-2"/>
+          <c:x val="0.0596364829396325"/>
           <c:y val="0.180094562647754"/>
-          <c:w val="0.89591907261592296"/>
-          <c:h val="0.56660337670557104"/>
+          <c:w val="0.895919072615923"/>
+          <c:h val="0.566603376705571"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1054,7 +1078,7 @@
                   <c:v>55.18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.590000000000003</c:v>
+                  <c:v>40.59</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>47.01</c:v>
@@ -1072,7 +1096,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F559-4290-95F1-ECCB1C0B378A}"/>
             </c:ext>
@@ -1109,7 +1133,7 @@
                   <c:v>43.37</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47</c:v>
+                  <c:v>47.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>56.18</c:v>
@@ -1124,7 +1148,7 @@
                   <c:v>35.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.299999999999997</c:v>
+                  <c:v>35.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>43.42</c:v>
@@ -1133,7 +1157,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F559-4290-95F1-ECCB1C0B378A}"/>
             </c:ext>
@@ -1148,11 +1172,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2142819488"/>
-        <c:axId val="-2142788960"/>
+        <c:axId val="613236832"/>
+        <c:axId val="662489632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2142819488"/>
+        <c:axId val="613236832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1191,10 +1215,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2142788960"/>
+        <c:crossAx val="662489632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1202,10 +1226,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2142788960"/>
+        <c:axId val="662489632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="30"/>
+          <c:min val="30.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1251,10 +1275,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2142819488"/>
+        <c:crossAx val="613236832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1293,7 +1317,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1323,7 +1347,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-BE"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1335,7 +1359,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
@@ -1374,6 +1398,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1399,7 +1424,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1439,99 +1464,99 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>15</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F9CB-4730-85D9-427D499DEA5E}"/>
             </c:ext>
@@ -1567,99 +1592,99 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>67</c:v>
+                  <c:v>67.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>60.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>59</c:v>
+                  <c:v>59.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>59</c:v>
+                  <c:v>59.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>57</c:v>
+                  <c:v>57.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90</c:v>
+                  <c:v>90.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>52</c:v>
+                  <c:v>52.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>53</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>54</c:v>
+                  <c:v>54.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>52</c:v>
+                  <c:v>52.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>62</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>68</c:v>
+                  <c:v>68.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>51</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>59</c:v>
+                  <c:v>59.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>53</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>96</c:v>
+                  <c:v>96.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>73</c:v>
+                  <c:v>73.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>61</c:v>
+                  <c:v>61.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>62</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>59</c:v>
+                  <c:v>59.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>65</c:v>
+                  <c:v>65.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>76</c:v>
+                  <c:v>76.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>61</c:v>
+                  <c:v>61.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F9CB-4730-85D9-427D499DEA5E}"/>
             </c:ext>
@@ -1673,11 +1698,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2121846256"/>
-        <c:axId val="-2140935264"/>
+        <c:axId val="680460512"/>
+        <c:axId val="620456736"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="2121846256"/>
+        <c:axId val="680460512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1716,10 +1741,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2140935264"/>
+        <c:crossAx val="620456736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1727,7 +1752,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2140935264"/>
+        <c:axId val="620456736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1775,10 +1800,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2121846256"/>
+        <c:crossAx val="680460512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1792,6 +1817,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1817,7 +1843,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1847,7 +1873,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-BE"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1859,7 +1885,409 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ansible</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ansible partial config'!$B$8:$AE$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>32.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Puppet</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ansible partial config'!$B$12:$AE$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="685722368"/>
+        <c:axId val="685728480"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="685722368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="685728480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="685728480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="685722368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.448229796933278"/>
+          <c:y val="0.884837416156314"/>
+          <c:w val="0.10645793617903"/>
+          <c:h val="0.0873848060659084"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
@@ -1904,6 +2332,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1929,7 +2358,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1982,7 +2411,7 @@
                   <c:v>5.68</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>11.18</c:v>
@@ -2030,7 +2459,7 @@
                   <c:v>8.23</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>7.41</c:v>
@@ -2039,7 +2468,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2C10-4E88-A46B-3E27751F553C}"/>
             </c:ext>
@@ -2080,7 +2509,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="stdDev"/>
             <c:noEndCap val="0"/>
-            <c:val val="1"/>
+            <c:val val="1.0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2102,70 +2531,70 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2C10-4E88-A46B-3E27751F553C}"/>
             </c:ext>
@@ -2181,11 +2610,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2097235968"/>
-        <c:axId val="-2097256496"/>
+        <c:axId val="655552192"/>
+        <c:axId val="655554512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2097235968"/>
+        <c:axId val="655552192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2224,10 +2653,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097256496"/>
+        <c:crossAx val="655554512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2235,7 +2664,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2097256496"/>
+        <c:axId val="655554512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2256,6 +2685,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2281,7 +2711,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="nl-BE"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2313,10 +2743,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097235968"/>
+        <c:crossAx val="655552192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2330,6 +2760,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2355,7 +2786,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2385,7 +2816,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-BE"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2396,8 +2827,8 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
@@ -2436,6 +2867,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2461,7 +2893,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2496,70 +2928,70 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>67</c:v>
+                  <c:v>67.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>60.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>59</c:v>
+                  <c:v>59.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>59</c:v>
+                  <c:v>59.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>57</c:v>
+                  <c:v>57.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90</c:v>
+                  <c:v>90.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>52</c:v>
+                  <c:v>52.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>53</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>54</c:v>
+                  <c:v>54.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>52</c:v>
+                  <c:v>52.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>62</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>68</c:v>
+                  <c:v>68.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>51</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>59</c:v>
+                  <c:v>59.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>53</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6CE5-4F04-A944-F1ECE6DD43AD}"/>
             </c:ext>
@@ -2602,7 +3034,7 @@
                   <c:v>55.18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.590000000000003</c:v>
+                  <c:v>40.59</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>47.01</c:v>
@@ -2653,7 +3085,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6CE5-4F04-A944-F1ECE6DD43AD}"/>
             </c:ext>
@@ -2668,11 +3100,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2097210768"/>
-        <c:axId val="-2097208448"/>
+        <c:axId val="578333424"/>
+        <c:axId val="578395088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2097210768"/>
+        <c:axId val="578333424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2711,10 +3143,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097208448"/>
+        <c:crossAx val="578395088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2722,7 +3154,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2097208448"/>
+        <c:axId val="578395088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2743,6 +3175,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2768,7 +3201,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="nl-BE"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2800,10 +3233,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097210768"/>
+        <c:crossAx val="578333424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2817,6 +3250,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2842,7 +3276,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2872,7 +3306,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-BE"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3083,6 +3517,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4637,7 +5111,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4745,6 +5219,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -4755,6 +5234,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -4786,6 +5270,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5140,6 +5627,509 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5675,7 +6665,7 @@
         <xdr:cNvPr id="6" name="Grafiek 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5711,7 +6701,7 @@
         <xdr:cNvPr id="7" name="Grafiek 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5752,7 +6742,7 @@
         <xdr:cNvPr id="2" name="Grafiek 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5777,6 +6767,41 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafiek 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
       <xdr:row>19</xdr:row>
@@ -5793,7 +6818,7 @@
         <xdr:cNvPr id="2" name="Grafiek 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5829,7 +6854,7 @@
         <xdr:cNvPr id="3" name="Grafiek 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5855,36 +6880,36 @@
   <autoFilter ref="A1:AE5"/>
   <tableColumns count="31">
     <tableColumn id="1" name="in seconden"/>
-    <tableColumn id="2" name="1" dataDxfId="30"/>
-    <tableColumn id="3" name="2" dataDxfId="29"/>
-    <tableColumn id="4" name="3" dataDxfId="28"/>
-    <tableColumn id="5" name="4" dataDxfId="27"/>
-    <tableColumn id="6" name="5" dataDxfId="26"/>
-    <tableColumn id="7" name="6" dataDxfId="25"/>
-    <tableColumn id="8" name="7" dataDxfId="24"/>
-    <tableColumn id="9" name="8" dataDxfId="23"/>
-    <tableColumn id="10" name="9" dataDxfId="22"/>
-    <tableColumn id="11" name="10" dataDxfId="21"/>
-    <tableColumn id="12" name="11" dataDxfId="20"/>
-    <tableColumn id="13" name="12" dataDxfId="19"/>
-    <tableColumn id="14" name="13" dataDxfId="18"/>
-    <tableColumn id="15" name="14" dataDxfId="17"/>
-    <tableColumn id="16" name="15" dataDxfId="16"/>
-    <tableColumn id="17" name="16" dataDxfId="15"/>
-    <tableColumn id="18" name="17" dataDxfId="14"/>
-    <tableColumn id="19" name="18" dataDxfId="13"/>
-    <tableColumn id="20" name="19" dataDxfId="12"/>
-    <tableColumn id="21" name="20" dataDxfId="11"/>
-    <tableColumn id="22" name="21" dataDxfId="10"/>
-    <tableColumn id="23" name="22" dataDxfId="9"/>
-    <tableColumn id="24" name="23" dataDxfId="8"/>
-    <tableColumn id="25" name="24" dataDxfId="7"/>
-    <tableColumn id="26" name="25" dataDxfId="6"/>
-    <tableColumn id="27" name="26" dataDxfId="5"/>
-    <tableColumn id="28" name="27" dataDxfId="4"/>
-    <tableColumn id="29" name="28" dataDxfId="3"/>
-    <tableColumn id="30" name="29" dataDxfId="2"/>
-    <tableColumn id="31" name="30" dataDxfId="1"/>
+    <tableColumn id="2" name="1" dataDxfId="31"/>
+    <tableColumn id="3" name="2" dataDxfId="30"/>
+    <tableColumn id="4" name="3" dataDxfId="29"/>
+    <tableColumn id="5" name="4" dataDxfId="28"/>
+    <tableColumn id="6" name="5" dataDxfId="27"/>
+    <tableColumn id="7" name="6" dataDxfId="26"/>
+    <tableColumn id="8" name="7" dataDxfId="25"/>
+    <tableColumn id="9" name="8" dataDxfId="24"/>
+    <tableColumn id="10" name="9" dataDxfId="23"/>
+    <tableColumn id="11" name="10" dataDxfId="22"/>
+    <tableColumn id="12" name="11" dataDxfId="21"/>
+    <tableColumn id="13" name="12" dataDxfId="20"/>
+    <tableColumn id="14" name="13" dataDxfId="19"/>
+    <tableColumn id="15" name="14" dataDxfId="18"/>
+    <tableColumn id="16" name="15" dataDxfId="17"/>
+    <tableColumn id="17" name="16" dataDxfId="16"/>
+    <tableColumn id="18" name="17" dataDxfId="15"/>
+    <tableColumn id="19" name="18" dataDxfId="14"/>
+    <tableColumn id="20" name="19" dataDxfId="13"/>
+    <tableColumn id="21" name="20" dataDxfId="12"/>
+    <tableColumn id="22" name="21" dataDxfId="11"/>
+    <tableColumn id="23" name="22" dataDxfId="10"/>
+    <tableColumn id="24" name="23" dataDxfId="9"/>
+    <tableColumn id="25" name="24" dataDxfId="8"/>
+    <tableColumn id="26" name="25" dataDxfId="7"/>
+    <tableColumn id="27" name="26" dataDxfId="6"/>
+    <tableColumn id="28" name="27" dataDxfId="5"/>
+    <tableColumn id="29" name="28" dataDxfId="4"/>
+    <tableColumn id="30" name="29" dataDxfId="3"/>
+    <tableColumn id="31" name="30" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5915,7 +6940,87 @@
     <tableColumn id="19" name="18"/>
     <tableColumn id="20" name="19"/>
     <tableColumn id="21" name="20"/>
+    <tableColumn id="22" name="21" dataDxfId="1"/>
+    <tableColumn id="23" name="22"/>
+    <tableColumn id="24" name="23"/>
+    <tableColumn id="25" name="24"/>
+    <tableColumn id="26" name="25"/>
+    <tableColumn id="27" name="26"/>
+    <tableColumn id="28" name="27"/>
+    <tableColumn id="29" name="28"/>
+    <tableColumn id="30" name="29"/>
+    <tableColumn id="31" name="30"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel24" displayName="Tabel24" ref="A2:AE4" totalsRowShown="0">
+  <autoFilter ref="A2:AE4"/>
+  <tableColumns count="31">
+    <tableColumn id="1" name="Kolom1"/>
+    <tableColumn id="2" name="1"/>
+    <tableColumn id="3" name="2"/>
+    <tableColumn id="4" name="3"/>
+    <tableColumn id="5" name="4"/>
+    <tableColumn id="6" name="5"/>
+    <tableColumn id="7" name="6"/>
+    <tableColumn id="8" name="7"/>
+    <tableColumn id="9" name="8"/>
+    <tableColumn id="10" name="9"/>
+    <tableColumn id="11" name="10"/>
+    <tableColumn id="12" name="11"/>
+    <tableColumn id="13" name="12"/>
+    <tableColumn id="14" name="13"/>
+    <tableColumn id="15" name="14"/>
+    <tableColumn id="16" name="15"/>
+    <tableColumn id="17" name="16"/>
+    <tableColumn id="18" name="17"/>
+    <tableColumn id="19" name="18"/>
+    <tableColumn id="20" name="19"/>
+    <tableColumn id="21" name="20"/>
     <tableColumn id="22" name="21" dataDxfId="0"/>
+    <tableColumn id="23" name="22"/>
+    <tableColumn id="24" name="23"/>
+    <tableColumn id="25" name="24"/>
+    <tableColumn id="26" name="25"/>
+    <tableColumn id="27" name="26"/>
+    <tableColumn id="28" name="27"/>
+    <tableColumn id="29" name="28"/>
+    <tableColumn id="30" name="29"/>
+    <tableColumn id="31" name="30"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel4" displayName="Tabel4" ref="A11:AE12" totalsRowShown="0">
+  <autoFilter ref="A11:AE12"/>
+  <tableColumns count="31">
+    <tableColumn id="1" name="Puppet"/>
+    <tableColumn id="2" name="1"/>
+    <tableColumn id="3" name="2"/>
+    <tableColumn id="4" name="3"/>
+    <tableColumn id="5" name="4"/>
+    <tableColumn id="6" name="5"/>
+    <tableColumn id="7" name="6"/>
+    <tableColumn id="8" name="7"/>
+    <tableColumn id="9" name="8"/>
+    <tableColumn id="10" name="9"/>
+    <tableColumn id="11" name="10"/>
+    <tableColumn id="12" name="11"/>
+    <tableColumn id="13" name="12"/>
+    <tableColumn id="14" name="13"/>
+    <tableColumn id="15" name="14"/>
+    <tableColumn id="16" name="15"/>
+    <tableColumn id="17" name="16"/>
+    <tableColumn id="18" name="17"/>
+    <tableColumn id="19" name="18"/>
+    <tableColumn id="20" name="19"/>
+    <tableColumn id="21" name="20"/>
+    <tableColumn id="22" name="21"/>
     <tableColumn id="23" name="22"/>
     <tableColumn id="24" name="23"/>
     <tableColumn id="25" name="24"/>
@@ -6195,16 +7300,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -6299,7 +7404,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -6394,7 +7499,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -6489,7 +7594,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -6602,7 +7707,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -6697,7 +7802,7 @@
         <v>51.3</v>
       </c>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -6714,7 +7819,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -6734,7 +7839,7 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -6751,7 +7856,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -6768,7 +7873,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -6785,7 +7890,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -6802,7 +7907,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -6819,7 +7924,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -6836,7 +7941,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -6853,7 +7958,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -6870,7 +7975,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -6887,7 +7992,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -6904,7 +8009,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -6921,42 +8026,42 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>13</v>
       </c>
@@ -6975,16 +8080,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE9"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6:AE6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.375" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -7079,7 +8184,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -7174,7 +8279,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -7269,13 +8374,13 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="V4" s="5"/>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="V5" s="5"/>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -7400,7 +8505,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -7525,7 +8630,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -7537,7 +8642,7 @@
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -7561,18 +8666,727 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="W2" t="s">
+        <v>47</v>
+      </c>
+      <c r="X2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>29</v>
+      </c>
+      <c r="E3">
+        <v>31</v>
+      </c>
+      <c r="F3">
+        <v>17</v>
+      </c>
+      <c r="G3">
+        <v>27</v>
+      </c>
+      <c r="H3">
+        <v>33</v>
+      </c>
+      <c r="I3">
+        <v>21</v>
+      </c>
+      <c r="J3">
+        <v>27</v>
+      </c>
+      <c r="K3">
+        <v>27</v>
+      </c>
+      <c r="L3">
+        <v>18</v>
+      </c>
+      <c r="M3">
+        <v>20</v>
+      </c>
+      <c r="N3">
+        <v>29</v>
+      </c>
+      <c r="O3">
+        <v>32</v>
+      </c>
+      <c r="P3">
+        <v>17</v>
+      </c>
+      <c r="Q3">
+        <v>19</v>
+      </c>
+      <c r="R3">
+        <v>19</v>
+      </c>
+      <c r="S3">
+        <v>26</v>
+      </c>
+      <c r="T3">
+        <v>24</v>
+      </c>
+      <c r="U3">
+        <v>31</v>
+      </c>
+      <c r="V3" s="5">
+        <v>22</v>
+      </c>
+      <c r="W3">
+        <v>21</v>
+      </c>
+      <c r="X3">
+        <v>29</v>
+      </c>
+      <c r="Y3">
+        <v>19</v>
+      </c>
+      <c r="Z3">
+        <v>20</v>
+      </c>
+      <c r="AA3">
+        <v>41</v>
+      </c>
+      <c r="AB3">
+        <v>20</v>
+      </c>
+      <c r="AC3">
+        <v>19</v>
+      </c>
+      <c r="AD3">
+        <v>31</v>
+      </c>
+      <c r="AE3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="5">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>23</v>
+      </c>
+      <c r="E4">
+        <v>23</v>
+      </c>
+      <c r="F4">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>19</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4">
+        <v>15</v>
+      </c>
+      <c r="J4">
+        <v>21</v>
+      </c>
+      <c r="K4">
+        <v>22</v>
+      </c>
+      <c r="L4" s="7">
+        <v>14</v>
+      </c>
+      <c r="M4" s="7">
+        <v>14</v>
+      </c>
+      <c r="N4" s="7">
+        <v>20</v>
+      </c>
+      <c r="O4" s="7">
+        <v>25</v>
+      </c>
+      <c r="P4" s="7">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>14</v>
+      </c>
+      <c r="R4">
+        <v>13</v>
+      </c>
+      <c r="S4">
+        <v>18</v>
+      </c>
+      <c r="T4" s="7">
+        <v>16</v>
+      </c>
+      <c r="U4">
+        <v>24</v>
+      </c>
+      <c r="V4" s="5">
+        <v>19</v>
+      </c>
+      <c r="W4">
+        <v>15</v>
+      </c>
+      <c r="X4">
+        <v>23</v>
+      </c>
+      <c r="Y4">
+        <v>13</v>
+      </c>
+      <c r="Z4">
+        <v>14</v>
+      </c>
+      <c r="AA4">
+        <v>32</v>
+      </c>
+      <c r="AB4">
+        <v>14</v>
+      </c>
+      <c r="AC4">
+        <v>14</v>
+      </c>
+      <c r="AD4">
+        <v>25</v>
+      </c>
+      <c r="AE4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="V5" s="5"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="V6" s="5"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="6">
+        <f t="shared" ref="B7:AE7" si="0">B3-B4</f>
+        <v>5</v>
+      </c>
+      <c r="C7" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G7" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I7" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K7" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L7" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M7" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="N7" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="O7" s="6">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="P7" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="Q7" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="R7" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="S7" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="T7" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="U7" s="6">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="V7" s="5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="W7" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="X7" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="Y7" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="Z7" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AA7" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="AB7" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AC7" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AD7" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AE7" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="6">
+        <f t="shared" ref="B8:AE8" si="1">B4</f>
+        <v>14</v>
+      </c>
+      <c r="C8" s="6">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D8" s="6">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="G8" s="6">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="J8" s="6">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="K8" s="6">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="L8" s="6">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="M8" s="6">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="N8" s="6">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="O8" s="6">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="P8" s="6">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="Q8" s="6">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="R8" s="6">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="S8" s="6">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="T8" s="6">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="U8" s="6">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="V8" s="5">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="W8" s="6">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="X8" s="6">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="Y8" s="6">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="Z8" s="6">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="AA8" s="6">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="AB8" s="6">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="AC8" s="6">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="AD8" s="6">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="AE8" s="6">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" t="s">
+        <v>29</v>
+      </c>
+      <c r="N11" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" t="s">
+        <v>31</v>
+      </c>
+      <c r="P11" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>33</v>
+      </c>
+      <c r="R11" t="s">
+        <v>34</v>
+      </c>
+      <c r="S11" t="s">
+        <v>35</v>
+      </c>
+      <c r="T11" t="s">
+        <v>36</v>
+      </c>
+      <c r="U11" t="s">
+        <v>37</v>
+      </c>
+      <c r="V11" t="s">
+        <v>46</v>
+      </c>
+      <c r="W11" t="s">
+        <v>47</v>
+      </c>
+      <c r="X11" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="21">
+    <row r="1" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
         <v>23</v>
       </c>
@@ -7583,7 +9397,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>43</v>
       </c>
@@ -7599,14 +9413,14 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>45</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>26</v>
       </c>
@@ -7619,7 +9433,7 @@
         <v>49.385333333333328</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>44</v>
       </c>
@@ -7632,7 +9446,7 @@
         <v>11.566646977359124</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
more results (deploy en enp0s8)
</commit_message>
<xml_diff>
--- a/R/deploytimes/deploytimes.xlsx
+++ b/R/deploytimes/deploytimes.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16040" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Puppet" sheetId="1" r:id="rId1"/>
     <sheet name="Ansible" sheetId="2" r:id="rId2"/>
     <sheet name="Ansible partial config" sheetId="5" r:id="rId3"/>
-    <sheet name="grafiek" sheetId="3" r:id="rId4"/>
+    <sheet name="no config" sheetId="6" r:id="rId4"/>
+    <sheet name="grafiek" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="64">
   <si>
     <t>total</t>
   </si>
@@ -217,6 +218,12 @@
   <si>
     <t>Puppet</t>
   </si>
+  <si>
+    <t>puppet verandfer zoalg github enkel de linen die veranderd zijn</t>
+  </si>
+  <si>
+    <t>(in seconden)</t>
+  </si>
 </sst>
 </file>
 
@@ -226,7 +233,7 @@
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -255,8 +262,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Andale Mono"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,6 +303,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -285,10 +319,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -300,8 +336,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="32">
@@ -464,6 +505,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -763,11 +805,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="680117488"/>
-        <c:axId val="680119264"/>
+        <c:axId val="366499792"/>
+        <c:axId val="366501568"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="680117488"/>
+        <c:axId val="366499792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -809,7 +851,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="680119264"/>
+        <c:crossAx val="366501568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -817,7 +859,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="680119264"/>
+        <c:axId val="366501568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -868,7 +910,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="680117488"/>
+        <c:crossAx val="366499792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -882,6 +924,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1172,11 +1215,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="613236832"/>
-        <c:axId val="662489632"/>
+        <c:axId val="365053456"/>
+        <c:axId val="365055776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="613236832"/>
+        <c:axId val="365053456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1218,7 +1261,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="662489632"/>
+        <c:crossAx val="365055776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1226,7 +1269,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="662489632"/>
+        <c:axId val="365055776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="30.0"/>
@@ -1278,7 +1321,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="613236832"/>
+        <c:crossAx val="365053456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1292,6 +1335,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1698,11 +1742,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="680460512"/>
-        <c:axId val="620456736"/>
+        <c:axId val="612756352"/>
+        <c:axId val="612758400"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="680460512"/>
+        <c:axId val="612756352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1744,7 +1788,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="620456736"/>
+        <c:crossAx val="612758400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1752,7 +1796,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="620456736"/>
+        <c:axId val="612758400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1803,7 +1847,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="680460512"/>
+        <c:crossAx val="612756352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1899,6 +1943,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-NL"/>
+              <a:t>deploytijd voor gedeeltelijke</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="nl-NL" baseline="0"/>
+              <a:t> configuratie</a:t>
+            </a:r>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2078,6 +2152,96 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>2.92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.91</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.86</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.93</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.88</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.24</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.36</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.93</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.97</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.96</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.87</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.87</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.87</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.09</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.93</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.96</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.93</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.88</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2092,11 +2256,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="685722368"/>
-        <c:axId val="685728480"/>
+        <c:axId val="613160128"/>
+        <c:axId val="612882048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="685722368"/>
+        <c:axId val="613160128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2138,7 +2302,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="685728480"/>
+        <c:crossAx val="612882048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2146,7 +2310,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="685728480"/>
+        <c:axId val="612882048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2196,7 +2360,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="685722368"/>
+        <c:crossAx val="613160128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2332,7 +2496,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2610,11 +2773,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="655552192"/>
-        <c:axId val="655554512"/>
+        <c:axId val="680405984"/>
+        <c:axId val="680379376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="655552192"/>
+        <c:axId val="680405984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2656,7 +2819,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="655554512"/>
+        <c:crossAx val="680379376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2664,7 +2827,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="655554512"/>
+        <c:axId val="680379376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2685,7 +2848,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2746,7 +2908,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="655552192"/>
+        <c:crossAx val="680405984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2760,7 +2922,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2867,7 +3028,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3100,11 +3260,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="578333424"/>
-        <c:axId val="578395088"/>
+        <c:axId val="613190640"/>
+        <c:axId val="613192960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="578333424"/>
+        <c:axId val="613190640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3146,7 +3306,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="578395088"/>
+        <c:crossAx val="613192960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3154,7 +3314,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="578395088"/>
+        <c:axId val="613192960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3175,7 +3335,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3236,7 +3395,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="578333424"/>
+        <c:crossAx val="613190640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3250,7 +3409,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8666,10 +8824,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE15"/>
+  <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AE13" sqref="AE13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9346,6 +9504,96 @@
       <c r="A12" t="s">
         <v>20</v>
       </c>
+      <c r="B12">
+        <v>2.92</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>2.96</v>
+      </c>
+      <c r="E12">
+        <v>2.98</v>
+      </c>
+      <c r="F12">
+        <v>2.91</v>
+      </c>
+      <c r="G12">
+        <v>5.86</v>
+      </c>
+      <c r="H12">
+        <v>3.11</v>
+      </c>
+      <c r="I12">
+        <v>2.93</v>
+      </c>
+      <c r="J12">
+        <v>2.88</v>
+      </c>
+      <c r="K12">
+        <v>3.24</v>
+      </c>
+      <c r="L12">
+        <v>3.19</v>
+      </c>
+      <c r="M12">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="N12">
+        <v>2.95</v>
+      </c>
+      <c r="O12">
+        <v>2.93</v>
+      </c>
+      <c r="P12">
+        <v>2.97</v>
+      </c>
+      <c r="Q12">
+        <v>2.9</v>
+      </c>
+      <c r="R12">
+        <v>2.96</v>
+      </c>
+      <c r="S12">
+        <v>2.85</v>
+      </c>
+      <c r="T12">
+        <v>2.95</v>
+      </c>
+      <c r="U12">
+        <v>2.87</v>
+      </c>
+      <c r="V12">
+        <v>2.87</v>
+      </c>
+      <c r="W12">
+        <v>2.87</v>
+      </c>
+      <c r="X12">
+        <v>3.09</v>
+      </c>
+      <c r="Y12">
+        <v>2.95</v>
+      </c>
+      <c r="Z12">
+        <v>2.93</v>
+      </c>
+      <c r="AA12">
+        <v>2.96</v>
+      </c>
+      <c r="AB12">
+        <v>2.93</v>
+      </c>
+      <c r="AC12">
+        <v>2.88</v>
+      </c>
+      <c r="AD12">
+        <v>2.8</v>
+      </c>
+      <c r="AE12">
+        <v>3.1</v>
+      </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -9360,6 +9608,11 @@
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -9374,6 +9627,264 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="11">
+        <v>0.41</v>
+      </c>
+      <c r="B2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
+        <v>0.38</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="11">
+        <v>0.34</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="12">
+        <v>0.37</v>
+      </c>
+      <c r="B5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="11">
+        <v>0.39</v>
+      </c>
+      <c r="B6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="12">
+        <v>0.38</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="12">
+        <v>0.43</v>
+      </c>
+      <c r="B9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="12">
+        <v>0.42</v>
+      </c>
+      <c r="B10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="12">
+        <v>0.38</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="12">
+        <v>0.62</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="12">
+        <v>0.38</v>
+      </c>
+      <c r="B14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="B15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="B16">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="12">
+        <v>0.35</v>
+      </c>
+      <c r="B18">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="12">
+        <v>0.42</v>
+      </c>
+      <c r="B19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="12">
+        <v>0.59</v>
+      </c>
+      <c r="B20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="12">
+        <v>0.39</v>
+      </c>
+      <c r="B21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="B22">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="12">
+        <v>0.38</v>
+      </c>
+      <c r="B23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="12">
+        <v>0.42</v>
+      </c>
+      <c r="B24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="12">
+        <v>0.44</v>
+      </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="12">
+        <v>0.44</v>
+      </c>
+      <c r="B26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="B27">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="12">
+        <v>0.42</v>
+      </c>
+      <c r="B29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="12">
+        <v>0.42</v>
+      </c>
+      <c r="B30">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E6"/>
   <sheetViews>

</xml_diff>

<commit_message>
methodology klaar voor revieuw
</commit_message>
<xml_diff>
--- a/R/deploytimes/deploytimes.xlsx
+++ b/R/deploytimes/deploytimes.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16040" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Puppet" sheetId="1" r:id="rId1"/>
     <sheet name="Ansible" sheetId="2" r:id="rId2"/>
-    <sheet name="Ansible partial config" sheetId="5" r:id="rId3"/>
-    <sheet name="no config" sheetId="6" r:id="rId4"/>
-    <sheet name="grafiek" sheetId="3" r:id="rId5"/>
+    <sheet name="Full config" sheetId="7" r:id="rId3"/>
+    <sheet name="Ansible partial config" sheetId="5" r:id="rId4"/>
+    <sheet name="no config" sheetId="6" r:id="rId5"/>
+    <sheet name="grafiek" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="84">
   <si>
     <t>total</t>
   </si>
@@ -224,6 +225,66 @@
   <si>
     <t>(in seconden)</t>
   </si>
+  <si>
+    <t>Z-toets: twee steekproeven voor gemiddelden</t>
+  </si>
+  <si>
+    <t>Variabele 1</t>
+  </si>
+  <si>
+    <t>Variabele 2</t>
+  </si>
+  <si>
+    <t>Gemiddelde</t>
+  </si>
+  <si>
+    <t>Bekende variantie</t>
+  </si>
+  <si>
+    <t>Waarnemingen</t>
+  </si>
+  <si>
+    <t>Schatting van verschil tussen gemiddelden</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>P(Z&lt;=z) eenzijdig</t>
+  </si>
+  <si>
+    <t>Kritiek gebied voor Z-toets: eenzijdig</t>
+  </si>
+  <si>
+    <t>P(Z&lt;=z) tweezijdig</t>
+  </si>
+  <si>
+    <t>Kritiek gebied voor Z-toets: tweezijdig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puppet </t>
+  </si>
+  <si>
+    <t>Ansible</t>
+  </si>
+  <si>
+    <t>gemiddelde</t>
+  </si>
+  <si>
+    <t>variatie</t>
+  </si>
+  <si>
+    <t>DEPLOY</t>
+  </si>
+  <si>
+    <t>Connectiontime</t>
+  </si>
+  <si>
+    <t>gemmidelde</t>
+  </si>
+  <si>
+    <t>afwijking</t>
+  </si>
 </sst>
 </file>
 
@@ -233,7 +294,7 @@
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -283,8 +344,16 @@
       <color theme="1"/>
       <name val="Andale Mono"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,13 +378,51 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -324,7 +431,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -339,6 +446,17 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -805,11 +923,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="366499792"/>
-        <c:axId val="366501568"/>
+        <c:axId val="704994912"/>
+        <c:axId val="748395936"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="366499792"/>
+        <c:axId val="704994912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -851,7 +969,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="366501568"/>
+        <c:crossAx val="748395936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -859,7 +977,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="366501568"/>
+        <c:axId val="748395936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -910,7 +1028,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="366499792"/>
+        <c:crossAx val="704994912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1215,11 +1333,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="365053456"/>
-        <c:axId val="365055776"/>
+        <c:axId val="746828336"/>
+        <c:axId val="747247296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="365053456"/>
+        <c:axId val="746828336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1261,7 +1379,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365055776"/>
+        <c:crossAx val="747247296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1269,7 +1387,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="365055776"/>
+        <c:axId val="747247296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="30.0"/>
@@ -1321,7 +1439,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365053456"/>
+        <c:crossAx val="746828336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1742,11 +1860,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="612756352"/>
-        <c:axId val="612758400"/>
+        <c:axId val="746802736"/>
+        <c:axId val="746805056"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="612756352"/>
+        <c:axId val="746802736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1788,7 +1906,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="612758400"/>
+        <c:crossAx val="746805056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1796,7 +1914,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="612758400"/>
+        <c:axId val="746805056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1847,7 +1965,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="612756352"/>
+        <c:crossAx val="746802736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1963,6 +2081,1154 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="nl-NL"/>
+              <a:t>deploytijd (volledige</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="nl-NL" baseline="0"/>
+              <a:t> configuratie)</a:t>
+            </a:r>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Puppet</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Puppet!$B$5:$AE$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>51.35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46.78</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55.18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>47.01</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.99</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.07</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43.29</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42.28</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>96.83</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32.33</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>49.99</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40.32</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>55.62</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>52.82</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42.72</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44.21</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43.13</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>47.43</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>56.98</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>59.97</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>61.28</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>53.98</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>56.56</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>53.57</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>49.01</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>50.21</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>51.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ansible</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Ansible!$B$7:$AE$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>73.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>61.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>61.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="775693616"/>
+        <c:axId val="775719536"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="775693616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="775719536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="775719536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>seconden</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="775693616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-NL"/>
+              <a:t>Connectietijd</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Puppet</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Puppet!$B$2:$AE$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.68</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.71</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.06</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.58</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.61</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.57</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.68</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.35</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.64</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.76</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.56</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.23</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.41</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ansible</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Ansible!$B$6:$AE$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="451352624"/>
+        <c:axId val="446959008"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="451352624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446959008"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="446959008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>seconden</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="451352624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-NL"/>
               <a:t>deploytijd voor gedeeltelijke</a:t>
             </a:r>
             <a:r>
@@ -2256,11 +3522,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="613160128"/>
-        <c:axId val="612882048"/>
+        <c:axId val="747982800"/>
+        <c:axId val="748091792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="613160128"/>
+        <c:axId val="747982800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2302,7 +3568,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="612882048"/>
+        <c:crossAx val="748091792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2310,7 +3576,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="612882048"/>
+        <c:axId val="748091792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2360,7 +3626,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="613160128"/>
+        <c:crossAx val="747982800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2450,7 +3716,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="nl-NL"/>
@@ -2496,6 +3762,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2773,11 +4040,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="680405984"/>
-        <c:axId val="680379376"/>
+        <c:axId val="705524320"/>
+        <c:axId val="705526640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="680405984"/>
+        <c:axId val="705524320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2819,7 +4086,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="680379376"/>
+        <c:crossAx val="705526640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2827,7 +4094,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="680379376"/>
+        <c:axId val="705526640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2848,6 +4115,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2908,7 +4176,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="680405984"/>
+        <c:crossAx val="705524320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2922,493 +4190,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="nl-NL"/>
-              <a:t>deploy</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Ansible (deploy)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Ansible!$B$7:$U$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>67.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>60.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>59.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>59.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>57.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>90.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>52.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>53.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>54.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>52.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>62.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>68.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>59.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>53.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>45.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6CE5-4F04-A944-F1ECE6DD43AD}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Puppet (deploy)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Puppet!$B$5:$U$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>51.35</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43.56</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>46.78</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>55.18</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40.59</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>47.01</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35.99</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35.07</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43.29</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>42.28</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>42.2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>96.83</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>32.33</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>49.99</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>40.32</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>55.62</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>52.82</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>42.72</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>44.21</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43.13</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6CE5-4F04-A944-F1ECE6DD43AD}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="613190640"/>
-        <c:axId val="613192960"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="613190640"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="613192960"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="613192960"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="nl-NL"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="613190640"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3715,6 +4497,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -5785,7 +6607,7 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5893,6 +6715,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -5903,6 +6730,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -5934,6 +6766,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6450,6 +7285,509 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6823,7 +8161,7 @@
         <xdr:cNvPr id="6" name="Grafiek 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6859,7 +8197,7 @@
         <xdr:cNvPr id="7" name="Grafiek 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6900,7 +8238,7 @@
         <xdr:cNvPr id="2" name="Grafiek 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6925,16 +8263,81 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafiek 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafiek 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>68036</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>181428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>126094</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>79828</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6956,19 +8359,19 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>196850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6976,7 +8379,7 @@
         <xdr:cNvPr id="2" name="Grafiek 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6989,42 +8392,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Grafiek 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7458,7 +8825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
@@ -8238,7 +9605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScale="69" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:K3"/>
     </sheetView>
   </sheetViews>
@@ -8824,10 +10191,167 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE33"/>
+  <dimension ref="C21:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AE13" sqref="AE13"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="58.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="J21" t="s">
+        <v>81</v>
+      </c>
+      <c r="K21" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="K22" s="22">
+        <f>AVERAGE(Puppet!B2:AE2)</f>
+        <v>8.2696666666666676</v>
+      </c>
+      <c r="L22" s="20">
+        <f>AVERAGE(Ansible!B6:AE6)</f>
+        <v>6.5666666666666664</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J23" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="K23" s="21">
+        <f>_xlfn.VAR.P(Puppet!B2:AE2)</f>
+        <v>4.1041165555555601</v>
+      </c>
+      <c r="L23" s="21">
+        <f>_xlfn.VAR.P(Ansible!B6:AE6)</f>
+        <v>6.112222222222222</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C24" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C25" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="14">
+        <v>49.385333333333328</v>
+      </c>
+      <c r="E25" s="14">
+        <v>60.666666666666664</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C26" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="14">
+        <v>129.32774499999999</v>
+      </c>
+      <c r="E26" s="14">
+        <v>127.88888900000001</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C27" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="14">
+        <v>30</v>
+      </c>
+      <c r="E27" s="14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C28" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="14">
+        <v>0</v>
+      </c>
+      <c r="E28" s="14"/>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C29" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="14">
+        <v>-3.8527562505248318</v>
+      </c>
+      <c r="E29" s="14"/>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C30" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="14">
+        <v>5.8397821801281502E-5</v>
+      </c>
+      <c r="E30" s="14"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C31" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="14">
+        <v>1.6448536269514715</v>
+      </c>
+      <c r="E31" s="14"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C32" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="14">
+        <v>1.16795643602563E-4</v>
+      </c>
+      <c r="E32" s="14"/>
+    </row>
+    <row r="33" spans="3:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" s="15">
+        <v>1.9599639845400536</v>
+      </c>
+      <c r="E33" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9610,9 +11134,44 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D35" s="19"/>
+      <c r="E35" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D36" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E36" s="19">
+        <f>AVERAGE(B8:AE8)</f>
+        <v>19.100000000000001</v>
+      </c>
+      <c r="F36" s="19">
+        <f>AVERAGE(Tabel4[[1]:[30]])</f>
+        <v>3.1033333333333335</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>79</v>
+      </c>
+      <c r="E37">
+        <f>VAR(B8:AE8)</f>
+        <v>33.403448275862097</v>
+      </c>
+      <c r="F37">
+        <f>VAR(Tabel4[[1]:[30]])</f>
+        <v>0.34594712643677761</v>
       </c>
     </row>
   </sheetData>
@@ -9626,17 +11185,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:B30"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="42.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -9647,7 +11210,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>0.41</v>
       </c>
@@ -9655,7 +11218,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>0.38</v>
       </c>
@@ -9663,7 +11226,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>0.34</v>
       </c>
@@ -9671,7 +11234,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <v>0.37</v>
       </c>
@@ -9679,7 +11242,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>0.39</v>
       </c>
@@ -9687,15 +11250,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
         <v>0.38</v>
       </c>
       <c r="B7">
         <v>20</v>
       </c>
+      <c r="E7" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>0.4</v>
       </c>
@@ -9703,87 +11269,163 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <v>0.43</v>
       </c>
       <c r="B9">
         <v>11</v>
       </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <v>0.42</v>
       </c>
       <c r="B10">
         <v>16</v>
       </c>
+      <c r="E10" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="14">
+        <v>0.42586206896551732</v>
+      </c>
+      <c r="G10" s="14">
+        <v>14.413793103448276</v>
+      </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
         <v>0.38</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
+      <c r="E11" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="14">
+        <v>1.1975120000000001E-2</v>
+      </c>
+      <c r="G11" s="14">
+        <v>18.251213499999999</v>
+      </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
         <v>0.62</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
+      <c r="E12" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="14">
+        <v>29</v>
+      </c>
+      <c r="G12" s="14">
+        <v>29</v>
+      </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="12">
         <v>0.36</v>
       </c>
       <c r="B13">
         <v>10</v>
       </c>
+      <c r="E13" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="14">
+        <v>0</v>
+      </c>
+      <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="12">
         <v>0.38</v>
       </c>
       <c r="B14">
         <v>15</v>
       </c>
+      <c r="E14" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="17">
+        <v>-17.626422634232298</v>
+      </c>
+      <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="12">
         <v>0.36</v>
       </c>
       <c r="B15">
         <v>17</v>
       </c>
+      <c r="E15" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="14">
+        <v>0</v>
+      </c>
+      <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="12">
         <v>0.36</v>
       </c>
       <c r="B16">
         <v>19</v>
       </c>
+      <c r="E16" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="14">
+        <v>1.64485362695147</v>
+      </c>
+      <c r="G16" s="14"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
         <v>0.4</v>
       </c>
       <c r="B17">
         <v>15</v>
       </c>
+      <c r="E17" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="17">
+        <v>0</v>
+      </c>
+      <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>0.35</v>
       </c>
       <c r="B18">
         <v>22</v>
       </c>
+      <c r="E18" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="18">
+        <v>1.9599639845400536</v>
+      </c>
+      <c r="G18" s="15"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="12">
         <v>0.42</v>
       </c>
@@ -9791,7 +11433,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="12">
         <v>0.59</v>
       </c>
@@ -9799,7 +11441,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="12">
         <v>0.39</v>
       </c>
@@ -9807,7 +11449,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="12">
         <v>0.4</v>
       </c>
@@ -9815,7 +11457,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="12">
         <v>0.38</v>
       </c>
@@ -9823,7 +11465,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="12">
         <v>0.42</v>
       </c>
@@ -9831,7 +11473,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="12">
         <v>0.44</v>
       </c>
@@ -9839,7 +11481,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="12">
         <v>0.44</v>
       </c>
@@ -9847,7 +11489,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="12">
         <v>0.4</v>
       </c>
@@ -9855,7 +11497,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="12">
         <v>0.9</v>
       </c>
@@ -9863,7 +11505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="12">
         <v>0.42</v>
       </c>
@@ -9871,7 +11513,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="12">
         <v>0.42</v>
       </c>
@@ -9881,14 +11523,15 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
transib periode tekst geschreven
</commit_message>
<xml_diff>
--- a/R/deploytimes/deploytimes.xlsx
+++ b/R/deploytimes/deploytimes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16040" tabRatio="500" activeTab="3"/>
+    <workbookView minimized="1" xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16040" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Puppet" sheetId="1" r:id="rId1"/>
@@ -923,11 +923,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="704994912"/>
-        <c:axId val="748395936"/>
+        <c:axId val="1881000528"/>
+        <c:axId val="1880261872"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="704994912"/>
+        <c:axId val="1881000528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -969,7 +969,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="748395936"/>
+        <c:crossAx val="1880261872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -977,7 +977,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="748395936"/>
+        <c:axId val="1880261872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1028,7 +1028,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="704994912"/>
+        <c:crossAx val="1881000528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1333,11 +1333,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="746828336"/>
-        <c:axId val="747247296"/>
+        <c:axId val="1884256672"/>
+        <c:axId val="1884258720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="746828336"/>
+        <c:axId val="1884256672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1379,7 +1379,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="747247296"/>
+        <c:crossAx val="1884258720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1387,7 +1387,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="747247296"/>
+        <c:axId val="1884258720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="30.0"/>
@@ -1439,7 +1439,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="746828336"/>
+        <c:crossAx val="1884256672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1860,11 +1860,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="746802736"/>
-        <c:axId val="746805056"/>
+        <c:axId val="1879863008"/>
+        <c:axId val="1879865328"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="746802736"/>
+        <c:axId val="1879863008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1906,7 +1906,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="746805056"/>
+        <c:crossAx val="1879865328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1914,7 +1914,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="746805056"/>
+        <c:axId val="1879865328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1965,7 +1965,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="746802736"/>
+        <c:crossAx val="1879863008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2091,7 +2091,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2374,11 +2373,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="775693616"/>
-        <c:axId val="775719536"/>
+        <c:axId val="1880280656"/>
+        <c:axId val="1838093888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="775693616"/>
+        <c:axId val="1880280656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2420,7 +2419,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="775719536"/>
+        <c:crossAx val="1838093888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2428,7 +2427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="775719536"/>
+        <c:axId val="1838093888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2474,7 +2473,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2534,7 +2532,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="775693616"/>
+        <c:crossAx val="1880280656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2662,7 +2660,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2937,7 +2934,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2946,11 +2942,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="451352624"/>
-        <c:axId val="446959008"/>
+        <c:axId val="1880764480"/>
+        <c:axId val="1880927616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="451352624"/>
+        <c:axId val="1880764480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2992,7 +2988,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="446959008"/>
+        <c:crossAx val="1880927616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3000,7 +2996,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="446959008"/>
+        <c:axId val="1880927616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3046,7 +3042,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3106,7 +3101,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451352624"/>
+        <c:crossAx val="1880764480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3522,11 +3517,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="747982800"/>
-        <c:axId val="748091792"/>
+        <c:axId val="1881063968"/>
+        <c:axId val="1881066288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="747982800"/>
+        <c:axId val="1881063968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3568,7 +3563,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="748091792"/>
+        <c:crossAx val="1881066288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3576,7 +3571,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="748091792"/>
+        <c:axId val="1881066288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3626,7 +3621,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="747982800"/>
+        <c:crossAx val="1881063968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3762,7 +3757,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4040,11 +4034,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="705524320"/>
-        <c:axId val="705526640"/>
+        <c:axId val="1880064656"/>
+        <c:axId val="1880066976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="705524320"/>
+        <c:axId val="1880064656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4086,7 +4080,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="705526640"/>
+        <c:crossAx val="1880066976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4094,7 +4088,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="705526640"/>
+        <c:axId val="1880066976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4115,7 +4109,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4176,7 +4169,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="705524320"/>
+        <c:crossAx val="1880064656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4190,7 +4183,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8161,7 +8153,7 @@
         <xdr:cNvPr id="6" name="Grafiek 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8197,7 +8189,7 @@
         <xdr:cNvPr id="7" name="Grafiek 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8238,7 +8230,7 @@
         <xdr:cNvPr id="2" name="Grafiek 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8379,7 +8371,7 @@
         <xdr:cNvPr id="2" name="Grafiek 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8825,8 +8817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="AG2" sqref="AG2"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection sqref="A1:AE5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9605,8 +9597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE9"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="69" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K3"/>
+    <sheetView topLeftCell="M1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:AF8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10350,8 +10342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36:E37"/>
+    <sheetView zoomScale="82" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:AE12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11189,8 +11181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="125" workbookViewId="0">
+      <selection sqref="A1:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>